<commit_message>
Active abilitys implemented without touch buttons
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\P_KiteEmAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84B5F74-11A3-4661-B323-A3A484D34F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D6E638-A9B9-49D5-A6FE-D6551C16DA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28770" yWindow="-5895" windowWidth="16230" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,33 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>bullet0,cosmic,geometric 2D, simple shapes, triangular, symmetric, sharp edges, game asset, vector graphic, solid color background,</t>
+  </si>
+  <si>
+    <t>shadows, gradient background</t>
+  </si>
+  <si>
+    <t>bullet,geometric, 2D, simple shapes, triangular, symmetric, sharp edges, game asset, vector graphic, solid color background</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -432,15 +456,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B37:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>